<commit_message>
Updated descriptive stuff for life history and wing methods
Made some updates to life history and wing methods. Regrouping on update stuff. Mostly table and image stuff
</commit_message>
<xml_diff>
--- a/lifehist/2017_08_28 R data descriptions.xlsx
+++ b/lifehist/2017_08_28 R data descriptions.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20625" windowHeight="7110" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20625" windowHeight="7110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data file definitions" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Field " sheetId="2" r:id="rId2"/>
+    <sheet name="Lab specifics" sheetId="3" r:id="rId3"/>
+    <sheet name="Lab summary" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="108">
   <si>
     <t>Type</t>
   </si>
@@ -335,13 +336,64 @@
   </si>
   <si>
     <t>Missing</t>
+  </si>
+  <si>
+    <t># Females</t>
+  </si>
+  <si>
+    <t># Males</t>
+  </si>
+  <si>
+    <r>
+      <t>Treatment- 20</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Treatment- 24</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Treatment- 28</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +408,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -772,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -855,6 +914,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -873,21 +941,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,7 +1295,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1245,7 +1312,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1327,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1275,7 +1342,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1290,7 +1357,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1305,7 +1372,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1320,7 +1387,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1335,7 +1402,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1417,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="46" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1365,7 +1432,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
@@ -1378,7 +1445,7 @@
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1393,7 +1460,7 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1406,7 +1473,7 @@
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1419,7 +1486,7 @@
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1432,7 +1499,7 @@
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1445,7 +1512,7 @@
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1458,7 +1525,7 @@
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1473,7 +1540,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1488,7 +1555,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="2" t="s">
         <v>71</v>
       </c>
@@ -1503,7 +1570,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
@@ -1518,7 +1585,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1533,7 +1600,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="2" t="s">
         <v>73</v>
       </c>
@@ -1548,7 +1615,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
@@ -1563,7 +1630,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
@@ -1578,14 +1645,14 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
-      <c r="B27" s="44" t="s">
+      <c r="A27" s="47"/>
+      <c r="B27" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="37" t="s">
         <v>75</v>
       </c>
       <c r="E27" s="13" t="s">
@@ -1608,7 +1675,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="Q2" sqref="Q2:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,10 +1810,10 @@
       <c r="O3" s="4">
         <v>40</v>
       </c>
-      <c r="P3" s="47">
+      <c r="P3" s="39">
         <v>44</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="49" t="s">
         <v>67</v>
       </c>
       <c r="R3" s="23" t="s">
@@ -1764,7 +1831,7 @@
       <c r="V3" s="26">
         <v>14</v>
       </c>
-      <c r="X3" s="48" t="s">
+      <c r="X3" s="40" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1807,7 +1874,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="43"/>
+      <c r="Q4" s="49"/>
       <c r="R4" s="27" t="s">
         <v>55</v>
       </c>
@@ -1873,7 +1940,7 @@
       <c r="P5" s="2">
         <v>42</v>
       </c>
-      <c r="Q5" s="43"/>
+      <c r="Q5" s="49"/>
       <c r="R5" s="27" t="s">
         <v>57</v>
       </c>
@@ -1939,7 +2006,7 @@
       <c r="P6" s="2">
         <v>43</v>
       </c>
-      <c r="Q6" s="43"/>
+      <c r="Q6" s="49"/>
       <c r="R6" s="27" t="s">
         <v>56</v>
       </c>
@@ -1969,7 +2036,7 @@
       <c r="D7" s="2">
         <v>12</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="41">
         <v>14</v>
       </c>
       <c r="F7" s="2"/>
@@ -1983,7 +2050,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="43" t="s">
+      <c r="Q7" s="49" t="s">
         <v>68</v>
       </c>
       <c r="R7" s="27" t="s">
@@ -2001,7 +2068,7 @@
       <c r="V7" s="30">
         <v>4</v>
       </c>
-      <c r="X7" s="50" t="s">
+      <c r="X7" s="42" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2040,7 +2107,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="43"/>
+      <c r="Q8" s="49"/>
       <c r="R8" s="27" t="s">
         <v>59</v>
       </c>
@@ -2118,7 +2185,7 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46">
+      <c r="A16" s="38">
         <v>42767</v>
       </c>
     </row>
@@ -2239,7 +2306,7 @@
       <c r="P18" s="4">
         <v>44</v>
       </c>
-      <c r="Q18" s="43" t="s">
+      <c r="Q18" s="49" t="s">
         <v>67</v>
       </c>
       <c r="R18" s="23" t="s">
@@ -2307,7 +2374,7 @@
       <c r="P19" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="Q19" s="43"/>
+      <c r="Q19" s="49"/>
       <c r="R19" s="27" t="s">
         <v>55</v>
       </c>
@@ -2373,7 +2440,7 @@
       <c r="P20" s="2">
         <v>42</v>
       </c>
-      <c r="Q20" s="43"/>
+      <c r="Q20" s="49"/>
       <c r="R20" s="27" t="s">
         <v>57</v>
       </c>
@@ -2439,7 +2506,7 @@
       <c r="P21" s="2">
         <v>43</v>
       </c>
-      <c r="Q21" s="43"/>
+      <c r="Q21" s="49"/>
       <c r="R21" s="27" t="s">
         <v>56</v>
       </c>
@@ -2474,18 +2541,18 @@
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="42" t="s">
+      <c r="H22" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
-      <c r="Q22" s="43" t="s">
+      <c r="Q22" s="49" t="s">
         <v>68</v>
       </c>
       <c r="R22" s="27" t="s">
@@ -2539,7 +2606,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="43"/>
+      <c r="Q23" s="49"/>
       <c r="R23" s="27" t="s">
         <v>59</v>
       </c>
@@ -2641,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,7 +2851,7 @@
         <v>88</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:I9" si="2">(F4/E4)*100</f>
+        <f t="shared" ref="G4:G9" si="2">(F4/E4)*100</f>
         <v>44.444444444444443</v>
       </c>
       <c r="H4">
@@ -4511,4 +4578,659 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+    </row>
+    <row r="3" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2">
+        <v>150</v>
+      </c>
+      <c r="D4" s="2">
+        <v>11</v>
+      </c>
+      <c r="E4" s="53">
+        <f>(D4/C4)</f>
+        <v>7.3333333333333334E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <f>G4+H4</f>
+        <v>134</v>
+      </c>
+      <c r="G4" s="2">
+        <v>65</v>
+      </c>
+      <c r="H4" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2">
+        <v>225</v>
+      </c>
+      <c r="D5" s="2">
+        <v>20</v>
+      </c>
+      <c r="E5" s="53">
+        <f t="shared" ref="E5:E10" si="0">(D5/C5)</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <f>G5+H5</f>
+        <v>198</v>
+      </c>
+      <c r="G5" s="2">
+        <v>88</v>
+      </c>
+      <c r="H5" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2">
+        <v>225</v>
+      </c>
+      <c r="D6" s="2">
+        <v>38</v>
+      </c>
+      <c r="E6" s="53">
+        <f t="shared" si="0"/>
+        <v>0.16888888888888889</v>
+      </c>
+      <c r="F6" s="2">
+        <f>G6+H6</f>
+        <v>181</v>
+      </c>
+      <c r="G6" s="2">
+        <v>89</v>
+      </c>
+      <c r="H6" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2">
+        <v>225</v>
+      </c>
+      <c r="D7" s="2">
+        <v>31</v>
+      </c>
+      <c r="E7" s="53">
+        <f t="shared" si="0"/>
+        <v>0.13777777777777778</v>
+      </c>
+      <c r="F7" s="2">
+        <f>G7+H7</f>
+        <v>192</v>
+      </c>
+      <c r="G7" s="2">
+        <v>102</v>
+      </c>
+      <c r="H7" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="2">
+        <v>120</v>
+      </c>
+      <c r="D8" s="2">
+        <v>29</v>
+      </c>
+      <c r="E8" s="53">
+        <f t="shared" si="0"/>
+        <v>0.24166666666666667</v>
+      </c>
+      <c r="F8" s="2">
+        <f>G8+H8</f>
+        <v>91</v>
+      </c>
+      <c r="G8" s="2">
+        <v>45</v>
+      </c>
+      <c r="H8" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="2">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2">
+        <v>27</v>
+      </c>
+      <c r="E9" s="53">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="F9" s="2">
+        <f>G9+H9</f>
+        <v>32</v>
+      </c>
+      <c r="G9" s="2">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2">
+        <v>165</v>
+      </c>
+      <c r="D10" s="2">
+        <v>31</v>
+      </c>
+      <c r="E10" s="53">
+        <f t="shared" si="0"/>
+        <v>0.18787878787878787</v>
+      </c>
+      <c r="F10" s="2">
+        <f>G10+H10</f>
+        <v>129</v>
+      </c>
+      <c r="G10" s="2">
+        <v>66</v>
+      </c>
+      <c r="H10" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+    </row>
+    <row r="13" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="2">
+        <v>150</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" s="53">
+        <f>(D14/C14)</f>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <f>G14+H14</f>
+        <v>135</v>
+      </c>
+      <c r="G14" s="2">
+        <v>57</v>
+      </c>
+      <c r="H14" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2">
+        <v>220</v>
+      </c>
+      <c r="D15" s="2">
+        <v>19</v>
+      </c>
+      <c r="E15" s="53">
+        <f t="shared" ref="E15:E20" si="1">(D15/C15)</f>
+        <v>8.6363636363636365E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <f>G15+H15</f>
+        <v>198</v>
+      </c>
+      <c r="G15" s="2">
+        <v>101</v>
+      </c>
+      <c r="H15" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="2">
+        <v>225</v>
+      </c>
+      <c r="D16" s="2">
+        <v>40</v>
+      </c>
+      <c r="E16" s="53">
+        <f t="shared" si="1"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="F16" s="2">
+        <f>G16+H16</f>
+        <v>184</v>
+      </c>
+      <c r="G16" s="2">
+        <v>98</v>
+      </c>
+      <c r="H16" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2">
+        <v>225</v>
+      </c>
+      <c r="D17" s="2">
+        <v>26</v>
+      </c>
+      <c r="E17" s="53">
+        <f t="shared" si="1"/>
+        <v>0.11555555555555555</v>
+      </c>
+      <c r="F17" s="2">
+        <f>G17+H17</f>
+        <v>197</v>
+      </c>
+      <c r="G17" s="2">
+        <v>96</v>
+      </c>
+      <c r="H17" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="2">
+        <v>120</v>
+      </c>
+      <c r="D18" s="2">
+        <v>34</v>
+      </c>
+      <c r="E18" s="53">
+        <f t="shared" si="1"/>
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="F18" s="2">
+        <f>G18+H18</f>
+        <v>84</v>
+      </c>
+      <c r="G18" s="2">
+        <v>41</v>
+      </c>
+      <c r="H18" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="2">
+        <v>55</v>
+      </c>
+      <c r="D19" s="2">
+        <v>20</v>
+      </c>
+      <c r="E19" s="53">
+        <f t="shared" si="1"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F19" s="2">
+        <f>G19+H19</f>
+        <v>35</v>
+      </c>
+      <c r="G19" s="2">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="2">
+        <v>165</v>
+      </c>
+      <c r="D20" s="2">
+        <v>36</v>
+      </c>
+      <c r="E20" s="53">
+        <f t="shared" si="1"/>
+        <v>0.21818181818181817</v>
+      </c>
+      <c r="F20" s="2">
+        <f>G20+H20</f>
+        <v>123</v>
+      </c>
+      <c r="G20" s="2">
+        <v>57</v>
+      </c>
+      <c r="H20" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="54"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+    </row>
+    <row r="23" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="2">
+        <v>150</v>
+      </c>
+      <c r="D24" s="2">
+        <v>16</v>
+      </c>
+      <c r="E24" s="53">
+        <f>(D24/C24)</f>
+        <v>0.10666666666666667</v>
+      </c>
+      <c r="F24" s="2">
+        <f>G24+H24</f>
+        <v>130</v>
+      </c>
+      <c r="G24" s="2">
+        <v>54</v>
+      </c>
+      <c r="H24" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="2">
+        <v>220</v>
+      </c>
+      <c r="D25" s="2">
+        <v>32</v>
+      </c>
+      <c r="E25" s="53">
+        <f t="shared" ref="E25:E30" si="2">(D25/C25)</f>
+        <v>0.14545454545454545</v>
+      </c>
+      <c r="F25" s="2">
+        <f>G25+H25</f>
+        <v>179</v>
+      </c>
+      <c r="G25" s="2">
+        <v>85</v>
+      </c>
+      <c r="H25" s="2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2">
+        <v>225</v>
+      </c>
+      <c r="D26" s="2">
+        <v>82</v>
+      </c>
+      <c r="E26" s="53">
+        <f t="shared" si="2"/>
+        <v>0.36444444444444446</v>
+      </c>
+      <c r="F26" s="2">
+        <f>G26+H26</f>
+        <v>141</v>
+      </c>
+      <c r="G26" s="2">
+        <v>65</v>
+      </c>
+      <c r="H26" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="2">
+        <v>225</v>
+      </c>
+      <c r="D27" s="2">
+        <v>62</v>
+      </c>
+      <c r="E27" s="53">
+        <f t="shared" si="2"/>
+        <v>0.27555555555555555</v>
+      </c>
+      <c r="F27" s="2">
+        <f>G27+H27</f>
+        <v>160</v>
+      </c>
+      <c r="G27" s="2">
+        <v>82</v>
+      </c>
+      <c r="H27" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2">
+        <v>120</v>
+      </c>
+      <c r="D28" s="2">
+        <v>49</v>
+      </c>
+      <c r="E28" s="53">
+        <f t="shared" si="2"/>
+        <v>0.40833333333333333</v>
+      </c>
+      <c r="F28" s="2">
+        <f>G28+H28</f>
+        <v>71</v>
+      </c>
+      <c r="G28" s="2">
+        <v>27</v>
+      </c>
+      <c r="H28" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="2">
+        <v>60</v>
+      </c>
+      <c r="D29" s="2">
+        <v>36</v>
+      </c>
+      <c r="E29" s="53">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="F29" s="2">
+        <f>G29+H29</f>
+        <v>24</v>
+      </c>
+      <c r="G29" s="2">
+        <v>10</v>
+      </c>
+      <c r="H29" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2">
+        <v>165</v>
+      </c>
+      <c r="D30" s="2">
+        <v>132</v>
+      </c>
+      <c r="E30" s="53">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="F30" s="2">
+        <f>G30+H30</f>
+        <v>33</v>
+      </c>
+      <c r="G30" s="2">
+        <v>16</v>
+      </c>
+      <c r="H30" s="2">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B22:H22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>